<commit_message>
calibrated with new camera with new height
</commit_message>
<xml_diff>
--- a/Calibration.xlsx
+++ b/Calibration.xlsx
@@ -32,7 +32,7 @@
     <t>mm Distance</t>
   </si>
   <si>
-    <t>height to the camera = 900 mm</t>
+    <t>height to the camera = 1340 mm</t>
   </si>
 </sst>
 </file>
@@ -372,85 +372,85 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="27"/>
                 <c:pt idx="0">
-                  <c:v>24</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>33</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>43</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>53</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>62</c:v>
-                </c:pt>
                 <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>72</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>82</c:v>
-                </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>92</c:v>
                 </c:pt>
-                <c:pt idx="8">
-                  <c:v>101</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>111</c:v>
-                </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>114</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>122</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="16">
                   <c:v>130</c:v>
                 </c:pt>
-                <c:pt idx="12">
-                  <c:v>140</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>150</c:v>
-                </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="17">
+                  <c:v>137</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>151</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>159</c:v>
                 </c:pt>
-                <c:pt idx="15">
-                  <c:v>170</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>177</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>187</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>196</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>206</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>219</c:v>
-                </c:pt>
                 <c:pt idx="21">
-                  <c:v>268</c:v>
+                  <c:v>193</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>317</c:v>
+                  <c:v>227</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>364</c:v>
+                  <c:v>264</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>413</c:v>
+                  <c:v>298</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>462</c:v>
+                  <c:v>333</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>512</c:v>
+                  <c:v>366</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1693,8 +1693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1716,7 +1716,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1724,7 +1724,7 @@
         <v>10</v>
       </c>
       <c r="B3" s="2">
-        <v>33</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1732,7 +1732,7 @@
         <v>20</v>
       </c>
       <c r="B4" s="2">
-        <v>43</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1740,7 +1740,7 @@
         <v>30</v>
       </c>
       <c r="B5" s="2">
-        <v>53</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1748,7 +1748,7 @@
         <v>40</v>
       </c>
       <c r="B6">
-        <v>62</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1756,7 +1756,7 @@
         <v>50</v>
       </c>
       <c r="B7">
-        <v>72</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1764,7 +1764,7 @@
         <v>60</v>
       </c>
       <c r="B8">
-        <v>82</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1772,7 +1772,7 @@
         <v>70</v>
       </c>
       <c r="B9">
-        <v>92</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1780,7 +1780,7 @@
         <v>80</v>
       </c>
       <c r="B10">
-        <v>101</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1788,7 +1788,7 @@
         <v>90</v>
       </c>
       <c r="B11">
-        <v>111</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -1796,7 +1796,7 @@
         <v>100</v>
       </c>
       <c r="B12">
-        <v>122</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -1804,7 +1804,7 @@
         <v>110</v>
       </c>
       <c r="B13">
-        <v>130</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -1812,7 +1812,7 @@
         <v>120</v>
       </c>
       <c r="B14">
-        <v>140</v>
+        <v>99</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -1820,7 +1820,7 @@
         <v>130</v>
       </c>
       <c r="B15">
-        <v>150</v>
+        <v>107</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -1828,7 +1828,7 @@
         <v>140</v>
       </c>
       <c r="B16">
-        <v>159</v>
+        <v>114</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1836,7 +1836,7 @@
         <v>150</v>
       </c>
       <c r="B17">
-        <v>170</v>
+        <v>122</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1844,7 +1844,7 @@
         <v>160</v>
       </c>
       <c r="B18">
-        <v>177</v>
+        <v>130</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1852,7 +1852,7 @@
         <v>170</v>
       </c>
       <c r="B19">
-        <v>187</v>
+        <v>137</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1860,7 +1860,7 @@
         <v>180</v>
       </c>
       <c r="B20">
-        <v>196</v>
+        <v>144</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1868,7 +1868,7 @@
         <v>190</v>
       </c>
       <c r="B21">
-        <v>206</v>
+        <v>151</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1876,7 +1876,7 @@
         <v>200</v>
       </c>
       <c r="B22">
-        <v>219</v>
+        <v>159</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1884,7 +1884,7 @@
         <v>250</v>
       </c>
       <c r="B23">
-        <v>268</v>
+        <v>193</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1892,7 +1892,7 @@
         <v>300</v>
       </c>
       <c r="B24">
-        <v>317</v>
+        <v>227</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1900,7 +1900,7 @@
         <v>350</v>
       </c>
       <c r="B25">
-        <v>364</v>
+        <v>264</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1908,7 +1908,7 @@
         <v>400</v>
       </c>
       <c r="B26">
-        <v>413</v>
+        <v>298</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1916,7 +1916,7 @@
         <v>450</v>
       </c>
       <c r="B27">
-        <v>462</v>
+        <v>333</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1924,7 +1924,7 @@
         <v>500</v>
       </c>
       <c r="B28">
-        <v>512</v>
+        <v>366</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>